<commit_message>
Feilretting, bl.a. manglende variable i spørring.
</commit_message>
<xml_diff>
--- a/doc/Nakke Bestillingsskjema, nye figurer.xlsx
+++ b/doc/Nakke Bestillingsskjema, nye figurer.xlsx
@@ -13,9 +13,9 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="353">
   <si>
     <t>Roker</t>
   </si>
@@ -1214,6 +1214,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Komplikasjoner, 3 mnd. etter operasjon</t>
   </si>
 </sst>
 </file>
@@ -1755,23 +1758,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Bestilling"/>
-      <sheetName val="Figurtyper"/>
-      <sheetName val="avklaringer"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2062,8 +2048,8 @@
   <dimension ref="A1:F158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="19" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="19" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3602,9 +3588,18 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="16"/>
-      <c r="D94" s="16"/>
-      <c r="E94" s="1"/>
+      <c r="A94" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="16"/>

</xml_diff>